<commit_message>
totul lucreaza din Excel file
</commit_message>
<xml_diff>
--- a/Excel/e.xlsx
+++ b/Excel/e.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://endava-my.sharepoint.com/personal/sorin_cucereavu_endava_com/Documents/Desktop/ReincarnareaATF/ReincarnareaATF/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sorin\Desktop\ReincarnareaATF\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_F25DC773A252ABDACC104816C99E50545ADE58EC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FB9DAF0E-D873-4F6B-B3F7-36311152B0E8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C59F13E0-E0BC-4C51-A328-748F42D57652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>username</t>
   </si>
@@ -33,7 +33,16 @@
     <t>pass</t>
   </si>
   <si>
-    <t>sorin</t>
+    <t>admin123</t>
+  </si>
+  <si>
+    <t>dan</t>
+  </si>
+  <si>
+    <t>ad123</t>
+  </si>
+  <si>
+    <t>Admin</t>
   </si>
 </sst>
 </file>
@@ -351,7 +360,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -369,10 +378,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>123</v>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>